<commit_message>
the labels need to chill
</commit_message>
<xml_diff>
--- a/Placement_Data_Full_Class.xlsx
+++ b/Placement_Data_Full_Class.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="7740"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -968,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O217"/>
+  <dimension ref="A1:O216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="E214" workbookViewId="0">
+      <selection activeCell="M225" sqref="M225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10941,12 +10941,6 @@
         <v>24</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O217">
-        <f>AVERAGE(O2:O216)</f>
-        <v>288655.40540540538</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>